<commit_message>
Add documentation and fix video error
</commit_message>
<xml_diff>
--- a/features/actionBlock.add.example.xlsx
+++ b/features/actionBlock.add.example.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
-    <t xml:space="preserve">BLOCK NAME</t>
+    <t xml:space="preserve">NAME</t>
   </si>
   <si>
     <t xml:space="preserve">DESCRIPTION</t>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">ACTION DISPLAY NAME    </t>
   </si>
   <si>
-    <t xml:space="preserve"> DETAILS      </t>
+    <t xml:space="preserve">ACTION DISPLAY DETAILS</t>
   </si>
   <si>
     <t xml:space="preserve">INPUT NAME</t>
@@ -459,8 +459,8 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="16.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -471,7 +471,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="31.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="22.3"/>
@@ -532,11 +532,11 @@
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="str">
         <f aca="false">"block " &amp; RANDBETWEEN(0,100000)</f>
-        <v>block 48817</v>
+        <v>block 43633</v>
       </c>
       <c r="B2" s="5" t="str">
         <f aca="false">"description " &amp; RANDBETWEEN(0,100000)</f>
-        <v>description 62868</v>
+        <v>description 34820</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>15</v>
@@ -555,7 +555,7 @@
       </c>
       <c r="H2" s="6" t="str">
         <f aca="false">"variable 1-" &amp; RANDBETWEEN(0,100000)</f>
-        <v>variable 1-56768</v>
+        <v>variable 1-16492</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>18</v>
@@ -568,7 +568,7 @@
       </c>
       <c r="L2" s="5" t="str">
         <f aca="false">"variable " &amp; RANDBETWEEN(0,100000)</f>
-        <v>variable 81462</v>
+        <v>variable 49167</v>
       </c>
       <c r="M2" s="7" t="s">
         <v>21</v>
@@ -583,11 +583,11 @@
     <row r="3" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="str">
         <f aca="false">"block " &amp; RANDBETWEEN(0,100000)</f>
-        <v>block 24020</v>
+        <v>block 75297</v>
       </c>
       <c r="B3" s="5" t="str">
         <f aca="false">"description " &amp; RANDBETWEEN(0,100000)</f>
-        <v>description 22551</v>
+        <v>description 37637</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>23</v>
@@ -606,7 +606,7 @@
       </c>
       <c r="H3" s="6" t="str">
         <f aca="false">"variable 2-" &amp; RANDBETWEEN(0,100000)</f>
-        <v>variable 2-61301</v>
+        <v>variable 2-40622</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>27</v>
@@ -619,7 +619,7 @@
       </c>
       <c r="L3" s="5" t="str">
         <f aca="false">"variable " &amp; RANDBETWEEN(0,100000)</f>
-        <v>variable 28020</v>
+        <v>variable 27455</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>30</v>
@@ -632,11 +632,11 @@
     <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="str">
         <f aca="false">"block " &amp; RANDBETWEEN(0,100000)</f>
-        <v>block 84831</v>
+        <v>block 25477</v>
       </c>
       <c r="B4" s="5" t="str">
         <f aca="false">"description " &amp; RANDBETWEEN(0,100000)</f>
-        <v>description 40425</v>
+        <v>description 2074</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>32</v>
@@ -655,33 +655,33 @@
       </c>
       <c r="H4" s="6" t="str">
         <f aca="false">"variable 3-" &amp; RANDBETWEEN(0,100000)</f>
-        <v>variable 3-33974</v>
+        <v>variable 3-62946</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>35</v>
       </c>
       <c r="J4" s="5" t="n">
         <f aca="true">RAND()*10</f>
-        <v>0.712005631843889</v>
+        <v>7.59517719132317</v>
       </c>
       <c r="K4" s="6" t="n">
         <f aca="false">J4</f>
-        <v>0.712005631843889</v>
+        <v>7.59517719132317</v>
       </c>
       <c r="L4" s="5" t="str">
         <f aca="false">"variable " &amp; RANDBETWEEN(0,100000)</f>
-        <v>variable 58258</v>
+        <v>variable 72035</v>
       </c>
       <c r="M4" s="7" t="s">
         <v>36</v>
       </c>
       <c r="N4" s="5" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
-        <v>788</v>
+        <v>890</v>
       </c>
       <c r="O4" s="6" t="n">
         <f aca="false">N4</f>
-        <v>788</v>
+        <v>890</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>